<commit_message>
Used git add then now using git commit
</commit_message>
<xml_diff>
--- a/Desktop/WBS.xlsx
+++ b/Desktop/WBS.xlsx
@@ -186,7 +186,7 @@
     <t>9/19 - 9/23</t>
   </si>
   <si>
-    <t>update</t>
+    <t>2nd update</t>
   </si>
 </sst>
 </file>
@@ -569,7 +569,7 @@
   <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="134" zoomScalePageLayoutView="134" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>